<commit_message>
Started working on project 02/04/2024
</commit_message>
<xml_diff>
--- a/SQL/mockup-for-sql.xlsx
+++ b/SQL/mockup-for-sql.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Learning-Testing\PyStrava\SQL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel Elizaldi\Desktop\Learning-Testing\PyStrava\SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E513C2A-20E4-43BC-A1D5-8A50DC298E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="All_Workouts_Table" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="77">
   <si>
     <t>activity_id</t>
   </si>
@@ -247,12 +246,18 @@
   </si>
   <si>
     <t>Total workouts as of July/05/2023</t>
+  </si>
+  <si>
+    <t>activity</t>
+  </si>
+  <si>
+    <t>activity_name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -326,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -336,6 +341,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,264 +558,178 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AH20"/>
+  <dimension ref="A1:AH21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="35.140625" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" customWidth="1"/>
-    <col min="18" max="18" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="35.109375" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" customWidth="1"/>
+    <col min="18" max="18" width="20.44140625" customWidth="1"/>
     <col min="19" max="19" width="11" customWidth="1"/>
-    <col min="20" max="21" width="35.140625" customWidth="1"/>
-    <col min="22" max="22" width="19.7109375" customWidth="1"/>
-    <col min="25" max="25" width="18.5703125" customWidth="1"/>
+    <col min="20" max="21" width="35.109375" customWidth="1"/>
+    <col min="22" max="22" width="19.6640625" customWidth="1"/>
+    <col min="25" max="25" width="18.5546875" customWidth="1"/>
     <col min="27" max="27" width="23" customWidth="1"/>
-    <col min="33" max="33" width="14.5703125" customWidth="1"/>
+    <col min="33" max="33" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="F2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="H2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" s="4" t="s">
+      <c r="N2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Y2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="Z2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AA2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AC2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AD2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AE2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AF2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="7" t="s">
+      <c r="AG2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="7" t="s">
+      <c r="AH2" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="3" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>10402560430</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B3" s="2">
         <v>45279</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="1">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>27.44</v>
-      </c>
-      <c r="I2" s="1">
-        <v>272</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1">
-        <v>30</v>
-      </c>
-      <c r="N2" s="1">
-        <v>130.19999999999999</v>
-      </c>
-      <c r="O2" s="1">
-        <v>155</v>
-      </c>
-      <c r="P2" s="1">
-        <v>4.43</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>0</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V2" s="1">
-        <v>1</v>
-      </c>
-      <c r="W2" s="1">
-        <v>20</v>
-      </c>
-      <c r="X2" s="1">
-        <v>25</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>15</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>15</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>35</v>
-      </c>
-      <c r="AD2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG2" s="1">
-        <v>115</v>
-      </c>
-      <c r="AH2" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>10396420409</v>
-      </c>
-      <c r="B3" s="2">
-        <v>45277</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E3" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
       </c>
       <c r="H3" s="1">
-        <v>19</v>
+        <v>27.44</v>
       </c>
       <c r="I3" s="1">
-        <v>159</v>
+        <v>272</v>
       </c>
       <c r="J3" s="1">
         <v>0</v>
@@ -819,16 +741,16 @@
         <v>0</v>
       </c>
       <c r="M3" s="1">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="N3" s="1">
-        <v>120.8</v>
+        <v>130.19999999999999</v>
       </c>
       <c r="O3" s="1">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="P3" s="1">
-        <v>3.56</v>
+        <v>4.43</v>
       </c>
       <c r="Q3" s="1">
         <v>0</v>
@@ -843,16 +765,16 @@
         <v>1</v>
       </c>
       <c r="W3" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="X3" s="1">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="Y3" s="1">
         <v>1</v>
       </c>
       <c r="Z3" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AA3" s="1">
         <v>15</v>
@@ -861,7 +783,7 @@
         <v>1</v>
       </c>
       <c r="AC3" s="1">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="AD3" s="1">
         <v>1</v>
@@ -873,39 +795,39 @@
         <v>0</v>
       </c>
       <c r="AG3" s="1">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="AH3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>10376354306</v>
+        <v>10396420409</v>
       </c>
       <c r="B4" s="2">
-        <v>45273</v>
+        <v>45277</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E4" s="1">
         <v>5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>20.309999999999999</v>
+        <v>19</v>
       </c>
       <c r="I4" s="1">
-        <v>243</v>
+        <v>159</v>
       </c>
       <c r="J4" s="1">
         <v>0</v>
@@ -917,16 +839,16 @@
         <v>0</v>
       </c>
       <c r="M4" s="1">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="N4" s="1">
-        <v>140.69999999999999</v>
+        <v>120.8</v>
       </c>
       <c r="O4" s="1">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="P4" s="1">
-        <v>3.77</v>
+        <v>3.56</v>
       </c>
       <c r="Q4" s="1">
         <v>0</v>
@@ -941,16 +863,16 @@
         <v>1</v>
       </c>
       <c r="W4" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="X4" s="1">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="Y4" s="1">
         <v>1</v>
       </c>
       <c r="Z4" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AA4" s="1">
         <v>15</v>
@@ -971,24 +893,24 @@
         <v>0</v>
       </c>
       <c r="AG4" s="1">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="AH4" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>10371196691</v>
+        <v>10376354306</v>
       </c>
       <c r="B5" s="2">
-        <v>45272</v>
+        <v>45273</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E5" s="1">
         <v>5</v>
@@ -1000,10 +922,10 @@
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <v>15.11</v>
+        <v>20.309999999999999</v>
       </c>
       <c r="I5" s="1">
-        <v>153</v>
+        <v>243</v>
       </c>
       <c r="J5" s="1">
         <v>0</v>
@@ -1015,16 +937,16 @@
         <v>0</v>
       </c>
       <c r="M5" s="1">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N5" s="1">
-        <v>128</v>
+        <v>140.69999999999999</v>
       </c>
       <c r="O5" s="1">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="P5" s="1">
-        <v>2.94</v>
+        <v>3.77</v>
       </c>
       <c r="Q5" s="1">
         <v>0</v>
@@ -1039,16 +961,16 @@
         <v>1</v>
       </c>
       <c r="W5" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="X5" s="1">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="Y5" s="1">
         <v>1</v>
       </c>
       <c r="Z5" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AA5" s="1">
         <v>15</v>
@@ -1069,39 +991,39 @@
         <v>0</v>
       </c>
       <c r="AG5" s="1">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="AH5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>10363350925</v>
+        <v>10371196691</v>
       </c>
       <c r="B6" s="2">
-        <v>45271</v>
+        <v>45272</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E6" s="1">
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
       </c>
       <c r="H6" s="1">
-        <v>25.59</v>
+        <v>15.11</v>
       </c>
       <c r="I6" s="1">
-        <v>270</v>
+        <v>153</v>
       </c>
       <c r="J6" s="1">
         <v>0</v>
@@ -1113,16 +1035,16 @@
         <v>0</v>
       </c>
       <c r="M6" s="1">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="N6" s="1">
-        <v>131.80000000000001</v>
+        <v>128</v>
       </c>
       <c r="O6" s="1">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="P6" s="1">
-        <v>5.1100000000000003</v>
+        <v>2.94</v>
       </c>
       <c r="Q6" s="1">
         <v>0</v>
@@ -1137,22 +1059,22 @@
         <v>1</v>
       </c>
       <c r="W6" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="X6" s="1">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="Y6" s="1">
         <v>1</v>
       </c>
       <c r="Z6" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AA6" s="1">
         <v>15</v>
       </c>
       <c r="AB6" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AC6" s="1">
         <v>25</v>
@@ -1167,24 +1089,24 @@
         <v>0</v>
       </c>
       <c r="AG6" s="1">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="AH6" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>10348140245</v>
+        <v>10363350925</v>
       </c>
       <c r="B7" s="2">
-        <v>45268</v>
+        <v>45271</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E7" s="1">
         <v>5</v>
@@ -1196,10 +1118,10 @@
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <v>24.19</v>
+        <v>25.59</v>
       </c>
       <c r="I7" s="1">
-        <v>220</v>
+        <v>270</v>
       </c>
       <c r="J7" s="1">
         <v>0</v>
@@ -1211,16 +1133,16 @@
         <v>0</v>
       </c>
       <c r="M7" s="1">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="N7" s="1">
-        <v>124.1</v>
+        <v>131.80000000000001</v>
       </c>
       <c r="O7" s="1">
         <v>157</v>
       </c>
       <c r="P7" s="1">
-        <v>4.6500000000000004</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="Q7" s="1">
         <v>0</v>
@@ -1235,7 +1157,7 @@
         <v>1</v>
       </c>
       <c r="W7" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="X7" s="1">
         <v>25</v>
@@ -1244,241 +1166,241 @@
         <v>1</v>
       </c>
       <c r="Z7" s="1">
+        <v>15</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>15</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>25</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>109</v>
+      </c>
+      <c r="AH7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>10348140245</v>
+      </c>
+      <c r="B8" s="2">
+        <v>45268</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>24.19</v>
+      </c>
+      <c r="I8" s="1">
+        <v>220</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>28</v>
+      </c>
+      <c r="N8" s="1">
+        <v>124.1</v>
+      </c>
+      <c r="O8" s="1">
+        <v>157</v>
+      </c>
+      <c r="P8" s="1">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="V8" s="1">
+        <v>1</v>
+      </c>
+      <c r="W8" s="1">
+        <v>15</v>
+      </c>
+      <c r="X8" s="1">
+        <v>25</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="1">
         <v>10</v>
       </c>
-      <c r="AA7" s="1">
-        <v>15</v>
-      </c>
-      <c r="AB7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC7" s="1">
-        <v>25</v>
-      </c>
-      <c r="AD7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="1">
+      <c r="AA8" s="1">
+        <v>15</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>25</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="1">
         <v>95</v>
       </c>
-      <c r="AH7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="AH8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>10343078755</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="2">
         <v>45267</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E9" s="1">
         <v>4</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G9" s="1">
         <v>3.01</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H9" s="1">
         <v>21.43</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I9" s="1">
         <v>228</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J9" s="1">
         <v>32</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K9" s="1">
         <v>8.3268000000000004</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L9" s="1">
         <v>14.3208</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M9" s="1">
         <v>23</v>
       </c>
-      <c r="N8" s="1">
+      <c r="N9" s="1">
         <v>131.19999999999999</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O9" s="1">
         <v>152</v>
       </c>
-      <c r="P8" s="1">
+      <c r="P9" s="1">
         <v>5.25</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="Q9" s="1">
         <v>7.07</v>
       </c>
-      <c r="R8" s="1">
+      <c r="R9" s="1">
         <v>30.400434834882599</v>
       </c>
-      <c r="S8" s="1">
+      <c r="S9" s="1">
         <v>-97.684114174917298</v>
       </c>
-      <c r="T8" s="1">
+      <c r="T9" s="1">
         <v>30.401210244744998</v>
       </c>
-      <c r="U8" s="1">
+      <c r="U9" s="1">
         <v>-97.684753881767307</v>
       </c>
-      <c r="V8" s="1">
-        <v>5</v>
-      </c>
-      <c r="W8" s="1">
-        <v>15</v>
-      </c>
-      <c r="X8" s="1">
-        <v>25</v>
-      </c>
-      <c r="Y8" s="1">
-        <v>5</v>
-      </c>
-      <c r="Z8" s="1">
-        <v>15</v>
-      </c>
-      <c r="AA8" s="1">
-        <v>15</v>
-      </c>
-      <c r="AB8" s="1">
-        <v>5</v>
-      </c>
-      <c r="AC8" s="1">
+      <c r="V9" s="1">
+        <v>5</v>
+      </c>
+      <c r="W9" s="1">
+        <v>15</v>
+      </c>
+      <c r="X9" s="1">
+        <v>25</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>15</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>15</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC9" s="1">
         <v>20</v>
       </c>
-      <c r="AD8" s="1">
-        <v>15</v>
-      </c>
-      <c r="AE8" s="1">
-        <v>15</v>
-      </c>
-      <c r="AF8" s="1">
+      <c r="AD9" s="1">
+        <v>15</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>15</v>
+      </c>
+      <c r="AF9" s="1">
         <v>10</v>
       </c>
-      <c r="AG8" s="1">
+      <c r="AG9" s="1">
         <v>135</v>
       </c>
-      <c r="AH8" s="1">
+      <c r="AH9" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+    <row r="10" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>10337763402</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
         <v>45266</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="1">
-        <v>5</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <v>29.47</v>
-      </c>
-      <c r="I9" s="1">
-        <v>217</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1">
-        <v>0</v>
-      </c>
-      <c r="L9" s="1">
-        <v>0</v>
-      </c>
-      <c r="M9" s="1">
-        <v>24</v>
-      </c>
-      <c r="N9" s="1">
-        <v>114.1</v>
-      </c>
-      <c r="O9" s="1">
-        <v>153</v>
-      </c>
-      <c r="P9" s="1">
-        <v>5.39</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>0</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V9" s="1">
-        <v>1</v>
-      </c>
-      <c r="W9" s="1">
-        <v>20</v>
-      </c>
-      <c r="X9" s="1">
-        <v>25</v>
-      </c>
-      <c r="Y9" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z9" s="1">
-        <v>10</v>
-      </c>
-      <c r="AA9" s="1">
-        <v>15</v>
-      </c>
-      <c r="AB9" s="1">
-        <v>5</v>
-      </c>
-      <c r="AC9" s="1">
-        <v>25</v>
-      </c>
-      <c r="AD9" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE9" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF9" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="1">
-        <v>104</v>
-      </c>
-      <c r="AH9" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>10332269232</v>
-      </c>
-      <c r="B10" s="2">
-        <v>45265</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>35</v>
@@ -1496,10 +1418,10 @@
         <v>0</v>
       </c>
       <c r="H10" s="1">
-        <v>41.35</v>
+        <v>29.47</v>
       </c>
       <c r="I10" s="1">
-        <v>246</v>
+        <v>217</v>
       </c>
       <c r="J10" s="1">
         <v>0</v>
@@ -1511,16 +1433,16 @@
         <v>0</v>
       </c>
       <c r="M10" s="1">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N10" s="1">
-        <v>105.6</v>
+        <v>114.1</v>
       </c>
       <c r="O10" s="1">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="P10" s="1">
-        <v>8.19</v>
+        <v>5.39</v>
       </c>
       <c r="Q10" s="1">
         <v>0</v>
@@ -1535,7 +1457,7 @@
         <v>1</v>
       </c>
       <c r="W10" s="1">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="X10" s="1">
         <v>25</v>
@@ -1565,78 +1487,72 @@
         <v>0</v>
       </c>
       <c r="AG10" s="1">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="AH10" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>10328994206</v>
+        <v>10332269232</v>
       </c>
       <c r="B11" s="2">
-        <v>45264</v>
+        <v>45265</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E11" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G11" s="1">
-        <v>2.6</v>
+        <v>0</v>
       </c>
       <c r="H11" s="1">
-        <v>42.49</v>
+        <v>41.35</v>
       </c>
       <c r="I11" s="1">
-        <v>202</v>
+        <v>246</v>
       </c>
       <c r="J11" s="1">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="K11" s="1">
-        <v>3.6503999999999999</v>
+        <v>0</v>
       </c>
       <c r="L11" s="1">
-        <v>14.781599999999999</v>
+        <v>0</v>
       </c>
       <c r="M11" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N11" s="1">
-        <v>84.5</v>
+        <v>105.6</v>
       </c>
       <c r="O11" s="1">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="P11" s="1">
-        <v>24.34</v>
+        <v>8.19</v>
       </c>
       <c r="Q11" s="1">
-        <v>16.21</v>
-      </c>
-      <c r="R11" s="1">
-        <v>30.4005054105073</v>
-      </c>
-      <c r="S11" s="1">
-        <v>-97.684128172695594</v>
-      </c>
-      <c r="T11" s="1">
-        <v>30.400525946169999</v>
-      </c>
-      <c r="U11" s="1">
-        <v>-97.683858862146707</v>
+        <v>0</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="V11" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W11" s="1">
         <v>35</v>
@@ -1645,402 +1561,408 @@
         <v>25</v>
       </c>
       <c r="Y11" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Z11" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AA11" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AB11" s="1">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="AC11" s="1">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="AD11" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AE11" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="AF11" s="1">
         <v>0</v>
       </c>
       <c r="AG11" s="1">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="AH11" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
+        <v>10328994206</v>
+      </c>
+      <c r="B12" s="2">
+        <v>45264</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="H12" s="1">
+        <v>42.49</v>
+      </c>
+      <c r="I12" s="1">
+        <v>202</v>
+      </c>
+      <c r="J12" s="1">
+        <v>48</v>
+      </c>
+      <c r="K12" s="1">
+        <v>3.6503999999999999</v>
+      </c>
+      <c r="L12" s="1">
+        <v>14.781599999999999</v>
+      </c>
+      <c r="M12" s="1">
+        <v>27</v>
+      </c>
+      <c r="N12" s="1">
+        <v>84.5</v>
+      </c>
+      <c r="O12" s="1">
+        <v>101</v>
+      </c>
+      <c r="P12" s="1">
+        <v>24.34</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>16.21</v>
+      </c>
+      <c r="R12" s="1">
+        <v>30.4005054105073</v>
+      </c>
+      <c r="S12" s="1">
+        <v>-97.684128172695594</v>
+      </c>
+      <c r="T12" s="1">
+        <v>30.400525946169999</v>
+      </c>
+      <c r="U12" s="1">
+        <v>-97.683858862146707</v>
+      </c>
+      <c r="V12" s="1">
+        <v>3</v>
+      </c>
+      <c r="W12" s="1">
+        <v>35</v>
+      </c>
+      <c r="X12" s="1">
+        <v>25</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>5</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>10</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>15</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>5</v>
+      </c>
+      <c r="AE12" s="1">
+        <v>15</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="1">
+        <v>123</v>
+      </c>
+      <c r="AH12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>10322687345</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B13" s="2">
         <v>45263</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E13" s="1">
         <v>21</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G13" s="1">
         <v>21.02</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H13" s="1">
         <v>123.16</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I13" s="1">
         <v>1698</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J13" s="1">
         <v>89</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K13" s="1">
         <v>10.231199999999999</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L13" s="1">
         <v>26.2836</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M13" s="1">
         <v>18</v>
       </c>
-      <c r="N12" s="1">
+      <c r="N13" s="1">
         <v>171.9</v>
       </c>
-      <c r="O12" s="1">
+      <c r="O13" s="1">
         <v>193</v>
       </c>
-      <c r="P12" s="1">
+      <c r="P13" s="1">
         <v>5.61</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="Q13" s="1">
         <v>5.52</v>
       </c>
-      <c r="R12" s="1">
+      <c r="R13" s="1">
         <v>29.4249127339571</v>
       </c>
-      <c r="S12" s="1">
+      <c r="S13" s="1">
         <v>-98.494579670950699</v>
       </c>
-      <c r="T12" s="1">
+      <c r="T13" s="1">
         <v>29.421691903844401</v>
       </c>
-      <c r="U12" s="1">
+      <c r="U13" s="1">
         <v>-98.499875776469693</v>
       </c>
-      <c r="V12" s="1">
+      <c r="V13" s="1">
         <v>30</v>
       </c>
-      <c r="W12" s="1">
+      <c r="W13" s="1">
         <v>50</v>
       </c>
-      <c r="X12" s="1">
+      <c r="X13" s="1">
         <v>100</v>
       </c>
-      <c r="Y12" s="1">
-        <v>5</v>
-      </c>
-      <c r="Z12" s="1">
+      <c r="Y13" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z13" s="1">
         <v>40</v>
       </c>
-      <c r="AA12" s="1">
+      <c r="AA13" s="1">
         <v>35</v>
       </c>
-      <c r="AB12" s="1">
-        <v>5</v>
-      </c>
-      <c r="AC12" s="1">
+      <c r="AB13" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC13" s="1">
         <v>35</v>
       </c>
-      <c r="AD12" s="1">
+      <c r="AD13" s="1">
         <v>30</v>
       </c>
-      <c r="AE12" s="1">
-        <v>25</v>
-      </c>
-      <c r="AF12" s="1">
-        <v>25</v>
-      </c>
-      <c r="AG12" s="1">
+      <c r="AE13" s="1">
+        <v>25</v>
+      </c>
+      <c r="AF13" s="1">
+        <v>25</v>
+      </c>
+      <c r="AG13" s="1">
         <v>355</v>
       </c>
-      <c r="AH12" s="1">
+      <c r="AH13" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+    <row r="14" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>10313897702</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B14" s="2">
         <v>45262</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="1">
-        <v>5</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1">
-        <v>26.27</v>
-      </c>
-      <c r="I13" s="1">
-        <v>270</v>
-      </c>
-      <c r="J13" s="1">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1">
-        <v>0</v>
-      </c>
-      <c r="L13" s="1">
-        <v>0</v>
-      </c>
-      <c r="M13" s="1">
-        <v>28</v>
-      </c>
-      <c r="N13" s="1">
-        <v>134.1</v>
-      </c>
-      <c r="O13" s="1">
-        <v>173</v>
-      </c>
-      <c r="P13" s="1">
-        <v>5.09</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>0</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V13" s="1">
-        <v>1</v>
-      </c>
-      <c r="W13" s="1">
-        <v>20</v>
-      </c>
-      <c r="X13" s="1">
-        <v>25</v>
-      </c>
-      <c r="Y13" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z13" s="1">
-        <v>15</v>
-      </c>
-      <c r="AA13" s="1">
-        <v>25</v>
-      </c>
-      <c r="AB13" s="1">
-        <v>5</v>
-      </c>
-      <c r="AC13" s="1">
-        <v>25</v>
-      </c>
-      <c r="AD13" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE13" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF13" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG13" s="1">
-        <v>119</v>
-      </c>
-      <c r="AH13" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>10309277702</v>
-      </c>
-      <c r="B14" s="2">
-        <v>45261</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E14" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="G14" s="1">
-        <v>2.02</v>
+        <v>0</v>
       </c>
       <c r="H14" s="1">
-        <v>15.28</v>
+        <v>26.27</v>
       </c>
       <c r="I14" s="1">
-        <v>153</v>
+        <v>270</v>
       </c>
       <c r="J14" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K14" s="1">
-        <v>7.8263999999999996</v>
+        <v>0</v>
       </c>
       <c r="L14" s="1">
-        <v>11.4732</v>
+        <v>0</v>
       </c>
       <c r="M14" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="N14" s="1">
-        <v>133.5</v>
+        <v>134.1</v>
       </c>
       <c r="O14" s="1">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="P14" s="1">
-        <v>7.4</v>
+        <v>5.09</v>
       </c>
       <c r="Q14" s="1">
-        <v>7.34</v>
-      </c>
-      <c r="R14" s="1">
-        <v>27.478308510035198</v>
-      </c>
-      <c r="S14" s="1">
-        <v>-99.487887499853898</v>
-      </c>
-      <c r="T14" s="1">
-        <v>27.479036813601802</v>
-      </c>
-      <c r="U14" s="1">
-        <v>-99.488604404032202</v>
+        <v>0</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="V14" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="W14" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="X14" s="1">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="Y14" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Z14" s="1">
         <v>15</v>
       </c>
       <c r="AA14" s="1">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="AB14" s="1">
         <v>5</v>
       </c>
       <c r="AC14" s="1">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="AD14" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="AE14" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="AF14" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AG14" s="1">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="AH14" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>10303798160</v>
+        <v>10309277702</v>
       </c>
       <c r="B15" s="2">
-        <v>45259</v>
+        <v>45261</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E15" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G15" s="1">
-        <v>0</v>
+        <v>2.02</v>
       </c>
       <c r="H15" s="1">
-        <v>15.33</v>
+        <v>15.28</v>
       </c>
       <c r="I15" s="1">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="J15" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K15" s="1">
-        <v>0</v>
+        <v>7.8263999999999996</v>
       </c>
       <c r="L15" s="1">
-        <v>0</v>
+        <v>11.4732</v>
       </c>
       <c r="M15" s="1">
         <v>25</v>
       </c>
       <c r="N15" s="1">
-        <v>137.19999999999999</v>
+        <v>133.5</v>
       </c>
       <c r="O15" s="1">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="P15" s="1">
-        <v>3.24</v>
+        <v>7.4</v>
       </c>
       <c r="Q15" s="1">
-        <v>0</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U15" s="1" t="s">
-        <v>36</v>
+        <v>7.34</v>
+      </c>
+      <c r="R15" s="1">
+        <v>27.478308510035198</v>
+      </c>
+      <c r="S15" s="1">
+        <v>-99.487887499853898</v>
+      </c>
+      <c r="T15" s="1">
+        <v>27.479036813601802</v>
+      </c>
+      <c r="U15" s="1">
+        <v>-99.488604404032202</v>
       </c>
       <c r="V15" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="W15" s="1">
         <v>10</v>
@@ -2049,7 +1971,7 @@
         <v>15</v>
       </c>
       <c r="Y15" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Z15" s="1">
         <v>15</v>
@@ -2058,78 +1980,78 @@
         <v>15</v>
       </c>
       <c r="AB15" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AC15" s="1">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="AD15" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="AE15" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="AF15" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AG15" s="1">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="AH15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>10298502876</v>
+        <v>10303798160</v>
       </c>
       <c r="B16" s="2">
         <v>45259</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E16" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G16" s="1">
-        <v>4.01</v>
+        <v>0</v>
       </c>
       <c r="H16" s="1">
-        <v>25</v>
+        <v>15.33</v>
       </c>
       <c r="I16" s="1">
-        <v>322</v>
+        <v>168</v>
       </c>
       <c r="J16" s="1">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="K16" s="1">
-        <v>9.6335999999999995</v>
+        <v>0</v>
       </c>
       <c r="L16" s="1">
-        <v>26.3232</v>
+        <v>0</v>
       </c>
       <c r="M16" s="1">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N16" s="1">
-        <v>152.6</v>
+        <v>137.19999999999999</v>
       </c>
       <c r="O16" s="1">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="P16" s="1">
-        <v>4.83</v>
+        <v>3.24</v>
       </c>
       <c r="Q16" s="1">
-        <v>6.14</v>
+        <v>0</v>
       </c>
       <c r="S16" s="1" t="s">
         <v>36</v>
@@ -2138,51 +2060,51 @@
         <v>36</v>
       </c>
       <c r="V16" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="W16" s="1">
+        <v>10</v>
+      </c>
+      <c r="X16" s="1">
+        <v>15</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>15</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>15</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC16" s="1">
         <v>20</v>
       </c>
-      <c r="X16" s="1">
-        <v>35</v>
-      </c>
-      <c r="Y16" s="1">
-        <v>5</v>
-      </c>
-      <c r="Z16" s="1">
-        <v>20</v>
-      </c>
-      <c r="AA16" s="1">
-        <v>25</v>
-      </c>
-      <c r="AB16" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC16" s="1">
-        <v>25</v>
-      </c>
       <c r="AD16" s="1">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="AE16" s="1">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="AF16" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AG16" s="1">
-        <v>186</v>
+        <v>80</v>
       </c>
       <c r="AH16" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>10292826019</v>
+        <v>10298502876</v>
       </c>
       <c r="B17" s="2">
-        <v>45258</v>
+        <v>45259</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>43</v>
@@ -2191,43 +2113,43 @@
         <v>47</v>
       </c>
       <c r="E17" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>48</v>
       </c>
       <c r="G17" s="1">
-        <v>6.01</v>
+        <v>4.01</v>
       </c>
       <c r="H17" s="1">
-        <v>44.09</v>
+        <v>25</v>
       </c>
       <c r="I17" s="1">
-        <v>475</v>
+        <v>322</v>
       </c>
       <c r="J17" s="1">
         <v>13</v>
       </c>
       <c r="K17" s="1">
-        <v>8.1684000000000001</v>
+        <v>9.6335999999999995</v>
       </c>
       <c r="L17" s="1">
-        <v>16.113600000000002</v>
+        <v>26.3232</v>
       </c>
       <c r="M17" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N17" s="1">
-        <v>146.4</v>
+        <v>152.6</v>
       </c>
       <c r="O17" s="1">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="P17" s="1">
-        <v>7.14</v>
+        <v>4.83</v>
       </c>
       <c r="Q17" s="1">
-        <v>7.2</v>
+        <v>6.14</v>
       </c>
       <c r="S17" s="1" t="s">
         <v>36</v>
@@ -2236,13 +2158,13 @@
         <v>36</v>
       </c>
       <c r="V17" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="W17" s="1">
+        <v>20</v>
+      </c>
+      <c r="X17" s="1">
         <v>35</v>
-      </c>
-      <c r="X17" s="1">
-        <v>40</v>
       </c>
       <c r="Y17" s="1">
         <v>5</v>
@@ -2254,78 +2176,78 @@
         <v>25</v>
       </c>
       <c r="AB17" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AC17" s="1">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="AD17" s="1">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="AE17" s="1">
+        <v>25</v>
+      </c>
+      <c r="AF17" s="1">
         <v>20</v>
       </c>
-      <c r="AF17" s="1">
-        <v>10</v>
-      </c>
       <c r="AG17" s="1">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="AH17" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>10275298329</v>
+        <v>10292826019</v>
       </c>
       <c r="B18" s="2">
-        <v>45254</v>
+        <v>45258</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E18" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G18" s="1">
-        <v>0</v>
+        <v>6.01</v>
       </c>
       <c r="H18" s="1">
-        <v>37.090000000000003</v>
+        <v>44.09</v>
       </c>
       <c r="I18" s="1">
-        <v>419</v>
+        <v>475</v>
       </c>
       <c r="J18" s="1">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="K18" s="1">
-        <v>0</v>
+        <v>8.1684000000000001</v>
       </c>
       <c r="L18" s="1">
-        <v>0</v>
+        <v>16.113600000000002</v>
       </c>
       <c r="M18" s="1">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="N18" s="1">
-        <v>146.30000000000001</v>
+        <v>146.4</v>
       </c>
       <c r="O18" s="1">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="P18" s="1">
-        <v>6.72</v>
+        <v>7.14</v>
       </c>
       <c r="Q18" s="1">
-        <v>0</v>
+        <v>7.2</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>36</v>
@@ -2334,16 +2256,16 @@
         <v>36</v>
       </c>
       <c r="V18" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="W18" s="1">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="X18" s="1">
         <v>40</v>
       </c>
       <c r="Y18" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Z18" s="1">
         <v>20</v>
@@ -2355,30 +2277,30 @@
         <v>5</v>
       </c>
       <c r="AC18" s="1">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="AD18" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="AE18" s="1">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="AF18" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AG18" s="1">
-        <v>149</v>
+        <v>210</v>
       </c>
       <c r="AH18" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>10263705407</v>
+        <v>10275298329</v>
       </c>
       <c r="B19" s="2">
-        <v>45252</v>
+        <v>45254</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>35</v>
@@ -2390,16 +2312,16 @@
         <v>5</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G19" s="1">
         <v>0</v>
       </c>
       <c r="H19" s="1">
-        <v>42.41</v>
+        <v>37.090000000000003</v>
       </c>
       <c r="I19" s="1">
-        <v>342</v>
+        <v>419</v>
       </c>
       <c r="J19" s="1">
         <v>0</v>
@@ -2411,16 +2333,16 @@
         <v>0</v>
       </c>
       <c r="M19" s="1">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="N19" s="1">
-        <v>127.4</v>
+        <v>146.30000000000001</v>
       </c>
       <c r="O19" s="1">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="P19" s="1">
-        <v>6.87</v>
+        <v>6.72</v>
       </c>
       <c r="Q19" s="1">
         <v>0</v>
@@ -2435,16 +2357,16 @@
         <v>1</v>
       </c>
       <c r="W19" s="1">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X19" s="1">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="Y19" s="1">
         <v>1</v>
       </c>
       <c r="Z19" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AA19" s="1">
         <v>25</v>
@@ -2465,126 +2387,227 @@
         <v>0</v>
       </c>
       <c r="AG19" s="1">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="AH19" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>10257445914</v>
+        <v>10263705407</v>
       </c>
       <c r="B20" s="2">
-        <v>45251</v>
+        <v>45252</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E20" s="1">
         <v>5</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G20" s="1">
-        <v>4.8600000000000003</v>
+        <v>0</v>
       </c>
       <c r="H20" s="1">
-        <v>31.57</v>
+        <v>42.41</v>
       </c>
       <c r="I20" s="1">
-        <v>393</v>
+        <v>342</v>
       </c>
       <c r="J20" s="1">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="K20" s="1">
-        <v>9.1188000000000002</v>
+        <v>0</v>
       </c>
       <c r="L20" s="1">
-        <v>16.315200000000001</v>
+        <v>0</v>
       </c>
       <c r="M20" s="1">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="N20" s="1">
-        <v>146.30000000000001</v>
+        <v>127.4</v>
       </c>
       <c r="O20" s="1">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="P20" s="1">
-        <v>6.15</v>
+        <v>6.87</v>
       </c>
       <c r="Q20" s="1">
-        <v>6.3</v>
-      </c>
-      <c r="R20" s="1">
-        <v>30.4011617135256</v>
-      </c>
-      <c r="S20" s="1">
-        <v>-97.684842562302904</v>
-      </c>
-      <c r="T20" s="1">
-        <v>30.401187110692199</v>
-      </c>
-      <c r="U20" s="1">
-        <v>-97.684776764362994</v>
+        <v>0</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="V20" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="W20" s="1">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="X20" s="1">
         <v>35</v>
       </c>
       <c r="Y20" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Z20" s="1">
+        <v>10</v>
+      </c>
+      <c r="AA20" s="1">
+        <v>25</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC20" s="1">
+        <v>25</v>
+      </c>
+      <c r="AD20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="1">
+        <v>139</v>
+      </c>
+      <c r="AH20" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>10257445914</v>
+      </c>
+      <c r="B21" s="2">
+        <v>45251</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="1">
+        <v>5</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="1">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="H21" s="1">
+        <v>31.57</v>
+      </c>
+      <c r="I21" s="1">
+        <v>393</v>
+      </c>
+      <c r="J21" s="1">
+        <v>40</v>
+      </c>
+      <c r="K21" s="1">
+        <v>9.1188000000000002</v>
+      </c>
+      <c r="L21" s="1">
+        <v>16.315200000000001</v>
+      </c>
+      <c r="M21" s="1">
+        <v>22</v>
+      </c>
+      <c r="N21" s="1">
+        <v>146.30000000000001</v>
+      </c>
+      <c r="O21" s="1">
+        <v>169</v>
+      </c>
+      <c r="P21" s="1">
+        <v>6.15</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>6.3</v>
+      </c>
+      <c r="R21" s="1">
+        <v>30.4011617135256</v>
+      </c>
+      <c r="S21" s="1">
+        <v>-97.684842562302904</v>
+      </c>
+      <c r="T21" s="1">
+        <v>30.401187110692199</v>
+      </c>
+      <c r="U21" s="1">
+        <v>-97.684776764362994</v>
+      </c>
+      <c r="V21" s="1">
+        <v>5</v>
+      </c>
+      <c r="W21" s="1">
+        <v>25</v>
+      </c>
+      <c r="X21" s="1">
+        <v>35</v>
+      </c>
+      <c r="Y21" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z21" s="1">
         <v>20</v>
       </c>
-      <c r="AA20" s="1">
-        <v>25</v>
-      </c>
-      <c r="AB20" s="1">
-        <v>5</v>
-      </c>
-      <c r="AC20" s="1">
-        <v>25</v>
-      </c>
-      <c r="AD20" s="1">
-        <v>25</v>
-      </c>
-      <c r="AE20" s="1">
+      <c r="AA21" s="1">
+        <v>25</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC21" s="1">
+        <v>25</v>
+      </c>
+      <c r="AD21" s="1">
+        <v>25</v>
+      </c>
+      <c r="AE21" s="1">
         <v>20</v>
       </c>
-      <c r="AF20" s="1">
+      <c r="AF21" s="1">
         <v>20</v>
       </c>
-      <c r="AG20" s="1">
+      <c r="AG21" s="1">
         <v>190</v>
       </c>
-      <c r="AH20" s="1">
+      <c r="AH21" s="1">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AH20">
+  <sortState ref="A2:AH20">
     <sortCondition descending="1" ref="B2:B20"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2595,13 +2618,13 @@
       <selection pane="bottomLeft" sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
@@ -2609,7 +2632,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>61</v>
       </c>
@@ -2617,7 +2640,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>62</v>
       </c>
@@ -2625,7 +2648,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>63</v>
       </c>
@@ -2633,7 +2656,7 @@
         <v>39.28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>64</v>
       </c>
@@ -2641,7 +2664,7 @@
         <v>427.5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>65</v>
       </c>
@@ -2649,7 +2672,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>66</v>
       </c>
@@ -2657,7 +2680,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>67</v>
       </c>
@@ -2665,7 +2688,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>68</v>
       </c>
@@ -2673,7 +2696,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>69</v>
       </c>
@@ -2681,7 +2704,7 @@
         <v>39.6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>70</v>
       </c>
@@ -2689,7 +2712,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>71</v>
       </c>
@@ -2703,7 +2726,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2714,12 +2737,12 @@
       <selection pane="bottomLeft" activeCell="B15" sqref="A1:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="27.42578125" customWidth="1"/>
+    <col min="1" max="2" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -2727,7 +2750,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
@@ -2735,7 +2758,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>43</v>
       </c>
@@ -2743,7 +2766,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>56</v>
       </c>
@@ -2751,7 +2774,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
@@ -2759,7 +2782,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -2767,7 +2790,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>53</v>
       </c>
@@ -2775,7 +2798,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -2783,7 +2806,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
@@ -2791,7 +2814,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>49</v>
       </c>
@@ -2799,7 +2822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
@@ -2807,7 +2830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -2815,7 +2838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
@@ -2823,7 +2846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>57</v>
       </c>
@@ -2831,7 +2854,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>74</v>
       </c>

</xml_diff>

<commit_message>
Finished working session 02/04/2024
</commit_message>
<xml_diff>
--- a/SQL/mockup-for-sql.xlsx
+++ b/SQL/mockup-for-sql.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="80">
   <si>
     <t>activity_id</t>
   </si>
@@ -257,7 +257,10 @@
     <t>activity_details</t>
   </si>
   <si>
-    <t>activity_</t>
+    <t>activity_coordinates</t>
+  </si>
+  <si>
+    <t>activity_scores</t>
   </si>
 </sst>
 </file>
@@ -337,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -357,6 +360,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -579,9 +585,9 @@
   </sheetPr>
   <dimension ref="A1:AH21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -632,6 +638,21 @@
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
       <c r="U1" s="5"/>
+      <c r="V1" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13"/>
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="13"/>
+      <c r="AG1" s="13"/>
+      <c r="AH1" s="13"/>
     </row>
     <row r="2" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2633,9 +2654,10 @@
   <sortState ref="A2:AH20">
     <sortCondition descending="1" ref="B2:B20"/>
   </sortState>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="F1:Q1"/>
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="V1:AH1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>